<commit_message>
menambahkan fitur update profil
</commit_message>
<xml_diff>
--- a/rancangan database.xlsx
+++ b/rancangan database.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_ver_7\xampp\htdocs\mijapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F497325C-215F-44FE-8B41-F8770D39DE66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D570346-4AAB-44AE-8BED-B6822D64C3F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
   <si>
     <t>id</t>
   </si>
@@ -201,9 +201,6 @@
     <t>divisi</t>
   </si>
   <si>
-    <t>divisi_kode</t>
-  </si>
-  <si>
     <t>user_divisi</t>
   </si>
   <si>
@@ -229,6 +226,27 @@
   </si>
   <si>
     <t>nip</t>
+  </si>
+  <si>
+    <t>id_karyawan</t>
+  </si>
+  <si>
+    <t>id_divisi</t>
+  </si>
+  <si>
+    <t>idkaryawan</t>
+  </si>
+  <si>
+    <t>kode_pos</t>
+  </si>
+  <si>
+    <t>kode_pos_domisili</t>
+  </si>
+  <si>
+    <t>ktp</t>
+  </si>
+  <si>
+    <t>fotoLama</t>
   </si>
 </sst>
 </file>
@@ -602,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,10 +652,10 @@
         <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>45</v>
@@ -656,13 +674,13 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
@@ -688,14 +706,14 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>67</v>
+      <c r="B3" t="s">
+        <v>66</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>58</v>
+      <c r="D3" t="s">
+        <v>57</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>67</v>
@@ -727,13 +745,13 @@
         <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>46</v>
@@ -749,17 +767,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
         <v>50</v>
@@ -772,17 +784,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
         <v>51</v>
@@ -796,7 +802,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
         <v>51</v>
@@ -807,7 +813,7 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
         <v>56</v>
@@ -818,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -832,163 +838,267 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menambahkan fitur menu lain dan subnya tanpa controller
</commit_message>
<xml_diff>
--- a/rancangan database.xlsx
+++ b/rancangan database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_ver_7\xampp\htdocs\mijapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D570346-4AAB-44AE-8BED-B6822D64C3F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0F9F7D-35AB-42CE-9A3F-7CF1943FD4C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>id</t>
   </si>
@@ -232,21 +232,6 @@
   </si>
   <si>
     <t>id_divisi</t>
-  </si>
-  <si>
-    <t>idkaryawan</t>
-  </si>
-  <si>
-    <t>kode_pos</t>
-  </si>
-  <si>
-    <t>kode_pos_domisili</t>
-  </si>
-  <si>
-    <t>ktp</t>
-  </si>
-  <si>
-    <t>fotoLama</t>
   </si>
 </sst>
 </file>
@@ -620,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,243 +847,139 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>27</v>
       </c>
-      <c r="D26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="D27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>29</v>
       </c>
-      <c r="D28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="D29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="D31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="D32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>34</v>
       </c>
-      <c r="D33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>35</v>
       </c>
-      <c r="D34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>36</v>
       </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="D36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>38</v>
       </c>
-      <c r="D37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>39</v>
       </c>
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>40</v>
       </c>
-      <c r="D39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>41</v>
       </c>
-      <c r="D40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>42</v>
       </c>
-      <c r="D41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>3</v>
       </c>
-      <c r="D42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>4</v>
-      </c>
-      <c r="D43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D46" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D47" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D48" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D49" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D50" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
berhasil menu tambah absen
</commit_message>
<xml_diff>
--- a/rancangan database.xlsx
+++ b/rancangan database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_ver_7\xampp\htdocs\mijapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574E0159-8330-4DD8-B7D8-3E9FB2B10A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B33FFE7-A1AF-4D9E-88D7-E7815F56FE5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>id</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>controller</t>
+  </si>
+  <si>
+    <t>cuti</t>
+  </si>
+  <si>
+    <t>hadir</t>
+  </si>
+  <si>
+    <t>user_update</t>
   </si>
 </sst>
 </file>
@@ -257,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +315,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -319,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -328,6 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,7 +627,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +710,7 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -706,8 +722,8 @@
       <c r="E3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>67</v>
+      <c r="F3" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>9</v>
@@ -739,7 +755,7 @@
         <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>46</v>
@@ -759,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H5" t="s">
         <v>49</v>
@@ -776,7 +792,7 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
         <v>50</v>
@@ -790,7 +806,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
         <v>51</v>
@@ -804,7 +820,7 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
         <v>56</v>
@@ -815,32 +831,47 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>11</v>
       </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>12</v>
       </c>
+      <c r="F11" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
menambah submenu user role akses
</commit_message>
<xml_diff>
--- a/rancangan database.xlsx
+++ b/rancangan database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_ver_7\xampp\htdocs\mijapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B33FFE7-A1AF-4D9E-88D7-E7815F56FE5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63994D2-A8BF-4A8A-A9B7-5F3D44F4897A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
   <si>
     <t>id</t>
   </si>
@@ -244,6 +244,63 @@
   </si>
   <si>
     <t>user_update</t>
+  </si>
+  <si>
+    <t>Tahun Ajaran</t>
+  </si>
+  <si>
+    <t>kelas</t>
+  </si>
+  <si>
+    <t>rombel</t>
+  </si>
+  <si>
+    <t>siswa</t>
+  </si>
+  <si>
+    <t>siswa_rombel</t>
+  </si>
+  <si>
+    <t>kode_kelas</t>
+  </si>
+  <si>
+    <t>nama_kelas</t>
+  </si>
+  <si>
+    <t>nama_rombel</t>
+  </si>
+  <si>
+    <t>id_kelas</t>
+  </si>
+  <si>
+    <t>id_siswa</t>
+  </si>
+  <si>
+    <t>id_rombel</t>
+  </si>
+  <si>
+    <t>jurnal_siswa</t>
+  </si>
+  <si>
+    <t>deskripsi</t>
+  </si>
+  <si>
+    <t>tindakan</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>kategori</t>
+  </si>
+  <si>
+    <t>id_kategori_jurnal</t>
+  </si>
+  <si>
+    <t>kategori_jurnal</t>
+  </si>
+  <si>
+    <t>aktif</t>
   </si>
 </sst>
 </file>
@@ -266,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +378,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -334,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -344,6 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="N6" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,13 +700,14 @@
     <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="18.88671875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -662,19 +727,40 @@
         <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -696,7 +782,7 @@
       <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
@@ -705,8 +791,29 @@
       <c r="J2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -725,20 +832,38 @@
       <c r="F3" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="O3" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -754,132 +879,171 @@
       <c r="E4" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" t="s">
+        <v>83</v>
+      </c>
+      <c r="M4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" t="s">
+      <c r="O4" t="s">
         <v>69</v>
       </c>
-      <c r="I4" t="s">
+      <c r="P4" t="s">
         <v>53</v>
       </c>
-      <c r="J4" t="s">
+      <c r="Q4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
         <v>51</v>
       </c>
-      <c r="J5" t="s">
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" t="s">
+        <v>89</v>
+      </c>
+      <c r="O6" t="s">
         <v>50</v>
       </c>
-      <c r="J6" t="s">
+      <c r="Q6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" t="s">
         <v>51</v>
       </c>
-      <c r="J7" t="s">
+      <c r="Q7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="M9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
revisi sampai menu pegawai
</commit_message>
<xml_diff>
--- a/rancangan database.xlsx
+++ b/rancangan database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_ver_7\xampp\htdocs\mijapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BEB48A-14B0-411A-AADA-EB40FF6BE1FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C20B69-5C99-42A1-84F6-0024396D2245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
menambah menu import siswa
</commit_message>
<xml_diff>
--- a/rancangan database.xlsx
+++ b/rancangan database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_ver_7\xampp\htdocs\mijapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C20B69-5C99-42A1-84F6-0024396D2245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55F7387-44C9-42C4-9912-1DF64AB3124E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
   <si>
     <t>id</t>
   </si>
@@ -252,12 +252,6 @@
     <t>siswa</t>
   </si>
   <si>
-    <t>siswa_rombel</t>
-  </si>
-  <si>
-    <t>id_siswa</t>
-  </si>
-  <si>
     <t>id_rombel</t>
   </si>
   <si>
@@ -289,6 +283,48 @@
   </si>
   <si>
     <t>id_kelas</t>
+  </si>
+  <si>
+    <t>nik</t>
+  </si>
+  <si>
+    <t>nisn</t>
+  </si>
+  <si>
+    <t>alamat</t>
+  </si>
+  <si>
+    <t>no_hp</t>
+  </si>
+  <si>
+    <t>ayah</t>
+  </si>
+  <si>
+    <t>pekerjaan_ayah</t>
+  </si>
+  <si>
+    <t>pendapatan_ayah</t>
+  </si>
+  <si>
+    <t>ibu</t>
+  </si>
+  <si>
+    <t>pekerjaan_ibu</t>
+  </si>
+  <si>
+    <t>pendapatan_ibu</t>
+  </si>
+  <si>
+    <t>tahun_lulus</t>
+  </si>
+  <si>
+    <t>lanjut_sekolah</t>
+  </si>
+  <si>
+    <t>last_user_update</t>
+  </si>
+  <si>
+    <t>panggilan</t>
   </si>
 </sst>
 </file>
@@ -690,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,14 +737,14 @@
     <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="18.88671875" customWidth="1"/>
-    <col min="13" max="13" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="18.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -737,28 +773,25 @@
         <v>74</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -780,7 +813,7 @@
       <c r="G2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
@@ -795,20 +828,17 @@
       <c r="L2" t="s">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -833,29 +863,29 @@
       <c r="H3" t="s">
         <v>73</v>
       </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="K3" t="s">
-        <v>82</v>
-      </c>
-      <c r="L3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N3" t="s">
+      <c r="M3" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -872,244 +902,313 @@
         <v>66</v>
       </c>
       <c r="F4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="M4" t="s">
+        <v>67</v>
+      </c>
       <c r="N4" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="O4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>59</v>
       </c>
-      <c r="L5" t="s">
+      <c r="I5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" t="s">
         <v>72</v>
       </c>
+      <c r="M5" t="s">
+        <v>49</v>
+      </c>
       <c r="N5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" t="s">
         <v>49</v>
       </c>
-      <c r="O5" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
         <v>60</v>
       </c>
-      <c r="L6" t="s">
+      <c r="I6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" t="s">
         <v>73</v>
       </c>
-      <c r="N6" t="s">
+      <c r="M6" t="s">
         <v>50</v>
       </c>
-      <c r="P6" t="s">
+      <c r="O6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>57</v>
       </c>
       <c r="E7" t="s">
         <v>61</v>
       </c>
-      <c r="L7" t="s">
-        <v>83</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" t="s">
         <v>51</v>
       </c>
-      <c r="P7" t="s">
+      <c r="O7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
         <v>62</v>
       </c>
-      <c r="L8" t="s">
-        <v>79</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="I8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
         <v>63</v>
       </c>
-      <c r="L9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
         <v>68</v>
       </c>
-      <c r="L10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="E12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I12" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I13" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>32</v>
       </c>

</xml_diff>